<commit_message>
Implement rank consistency measurement
</commit_message>
<xml_diff>
--- a/scripts/report/pairs-v5.xlsx
+++ b/scripts/report/pairs-v5.xlsx
@@ -1091,7 +1091,7 @@
         <v>40.04280223394357</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -2701,7 +2701,7 @@
         <v>36.20300882535897</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -3541,7 +3541,7 @@
         <v>36.20300882535897</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
@@ -4031,7 +4031,7 @@
         <v>36.20300882535897</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" t="b">
         <v>1</v>
@@ -5081,7 +5081,7 @@
         <v>50.5124584368011</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
@@ -5781,7 +5781,7 @@
         <v>40.04280223394357</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77" t="b">
         <v>0</v>
@@ -5851,7 +5851,7 @@
         <v>50.5124584368011</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
@@ -6061,7 +6061,7 @@
         <v>36.20300882535897</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
@@ -6761,7 +6761,7 @@
         <v>40.04280223394357</v>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" t="b">
         <v>0</v>
@@ -7181,7 +7181,7 @@
         <v>36.20300882535897</v>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" t="b">
         <v>1</v>
@@ -7251,7 +7251,7 @@
         <v>50.5124584368011</v>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" t="b">
         <v>0</v>
@@ -7461,7 +7461,7 @@
         <v>50.5124584368011</v>
       </c>
       <c r="F101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101" t="b">
         <v>0</v>
@@ -8861,7 +8861,7 @@
         <v>40.04280223394357</v>
       </c>
       <c r="F121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121" t="b">
         <v>0</v>
@@ -11591,7 +11591,7 @@
         <v>50.5124584368011</v>
       </c>
       <c r="F160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G160" t="b">
         <v>0</v>
@@ -12641,7 +12641,7 @@
         <v>36.20300882535897</v>
       </c>
       <c r="F175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G175" t="b">
         <v>1</v>
@@ -13271,7 +13271,7 @@
         <v>40.04280223394357</v>
       </c>
       <c r="F184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G184" t="b">
         <v>0</v>
@@ -13621,7 +13621,7 @@
         <v>40.04280223394357</v>
       </c>
       <c r="F189" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G189" t="b">
         <v>0</v>

</xml_diff>